<commit_message>
[CN] EP15 : Dissociative Recombination (TL Only)
</commit_message>
<xml_diff>
--- a/temp/temp.xlsx
+++ b/temp/temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AN-EN-Tags-NEW\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75CE7B1-AB28-4D21-9A63-57D2970595FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFF9348-A4E8-4BB8-868A-3F74C336F893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KW" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="244">
   <si>
     <t>Op</t>
   </si>
@@ -1784,35 +1784,81 @@
     <t>Cannot leave the field; will deploy at the target location with the current HP</t>
   </si>
   <si>
-    <t>Necrass</t>
-  </si>
-  <si>
-    <t>Wulfenite</t>
-  </si>
-  <si>
-    <t>Brigid</t>
-  </si>
-  <si>
-    <t>Thorns the Lodestar</t>
-  </si>
-  <si>
-    <t>Tin Man</t>
-  </si>
-  <si>
-    <t>Gnosis</t>
-  </si>
-  <si>
-    <t>Vigil</t>
-  </si>
-  <si>
-    <t>Saileach</t>
-  </si>
-  <si>
-    <t>Pozyomka</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Attacks from the 'Typewriter' reduce the target's DEF by </t>
+    <t>Mon3tr</t>
+  </si>
+  <si>
+    <t>Alanna</t>
+  </si>
+  <si>
+    <t>Windscoot</t>
+  </si>
+  <si>
+    <t>Ines</t>
+  </si>
+  <si>
+    <t>Cantabile</t>
+  </si>
+  <si>
+    <t>Puzzle</t>
+  </si>
+  <si>
+    <t>Surfer</t>
+  </si>
+  <si>
+    <t>Logos</t>
+  </si>
+  <si>
+    <t>Mudrock</t>
+  </si>
+  <si>
+    <t>Mod Trait</t>
+  </si>
+  <si>
+    <t>Trait</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The first hit on each enemy </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.root&gt;Binds&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the target for 5 seconds and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.steal&gt;Steals&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -1822,7 +1868,357 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>18%</t>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK (effect expires when enemy is defeated or Ines retreats)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The first hit on each enemy </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.root&gt;Binds&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the target for 5 seconds and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.steal&gt;Steals&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;(+10)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK (effect expires when enemy is defeated or Ines retreats)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ASPD +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when not blocking an enemy, ATK +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>% when blocking an enemy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ASPD +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;(+2)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when not blocking an enemy, ATK +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;(+2%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when blocking an enemy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ATK increased to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, recover 2 additional SP and reduce movement speed for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds when hitting an enemy with full HP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ATK increased to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;(+5%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, recover 2 additional SP and reduce movement speed for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds when hitting an enemy with full HP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When deployed, if there are no operators within the adjacent 4 tiles, gain 2 DP and ASPD + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
     </r>
     <r>
       <rPr>
@@ -1842,17 +2238,42 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds; if the 'Typewriter' is placed within the 4 tiles adjacent to Pozëmka, this effect increases to </t>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>When deployed, if there are no operators within the adjacent 4 tiles, gain 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;(+1)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DP and ASPD + </t>
     </r>
     <r>
       <rPr>
@@ -1862,12 +2283,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>23%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Attacks from the 'Typewriter' reduce the target's DEF by </t>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
     </r>
     <r>
       <rPr>
@@ -1877,7 +2303,77 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>20%</t>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When attacking a target, there is a 40% chance to deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Arts damage to 2 random targets in attack range and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.sluggish&gt;Slow&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> it for 0.8s.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When attacking a target, there is a 40% chance to deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
     </r>
     <r>
       <rPr>
@@ -1897,17 +2393,42 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.talpu&gt;(+2%)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for </t>
+      <t>&lt;@ba.talpu&gt;(+5%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Arts damage to 2 random targets in attack range and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.sluggish&gt;Slow&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> it for 0.8s.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Takes </t>
     </r>
     <r>
       <rPr>
@@ -1917,7 +2438,227 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>5</t>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> less damage from Sarkaz enemies and increase </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> damage to non-Sarkaz enemies</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Attack Range </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, target 2 enemies simultaneously. Attacks deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Physical damage and ignores their Physical Dodge </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ASPD + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and DEF + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When Trait effect reach maximum value, deals extra </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Physical damage on every attack</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ATK + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, ASPD + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and Talent effect. Gain 1 Support Device when the skill ends</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Has </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;reduced&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Redeployment Time, can use ranged attacks; Reduce the first retreat redeployment time by 35% </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Carries </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
     </r>
     <r>
       <rPr>
@@ -1932,22 +2673,172 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;Support Devices&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (max </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> deployed at once). Each </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;Support Devices&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> grants </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DEF ignore to an operator for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds (Effects do not stack)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Passive: Support Devices also grant ASPD+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. The Devices last </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds longer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Increases the heal amount of the next heal to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FF00B0FF"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.talpu&gt;(+1)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds; if the 'Typewriter' is placed within the 4 tiles adjacent to Pozëmka, this effect increases to </t>
+      <t>&lt;@ba.vup&gt;{heal_scale:0%}&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK, heal bounces </t>
     </r>
     <r>
       <rPr>
@@ -1957,1094 +2848,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.talpu&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>25%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(+2%)&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>Flagbearer</t>
-  </si>
-  <si>
-    <t>Alchemist</t>
-  </si>
-  <si>
-    <t>Mod Y</t>
-  </si>
-  <si>
-    <t>Mod X</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Gains </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Physical Dodge after attack </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> times</t>
-    </r>
-  </si>
-  <si>
-    <t>Necrass Tok skill</t>
-  </si>
-  <si>
-    <t>When there are alchemical units on the field, increase SP recovery rate by +0.1 SP/sec</t>
-  </si>
-  <si>
-    <r>
-      <t>ATK+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. When there are other operators within Attack Range, increase the duration of Alchemical units by </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ATK+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>14%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;(+4%)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. When there are other operators within Attack Range, increase the duration of Alchemical units by </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;(+1)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Increases the continuous damage dealt to ground enemies in range of Tin Man's Alchemical Units by </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Increases the continuous damage dealt to ground enemies in range of Tin Man's Alchemical Units by </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>22</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;(+2%)&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When a trap is triggered, if there are 2 or more enemies in trap range, increase damage by/to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{%}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Grants </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.buffres&gt;Resist&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and ATK </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+{%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to all </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Karlan Trade]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Operators after Gnosis has been deployed for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Vigil and the Wolfpack's attacks ignore </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>175</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DEF when attacking enemies blocked by the Wolfpack and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.steal&gt;Steal&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{def_steal}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DEF from the target (Caps at </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{def_steal_max}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Vigil and the Wolfpack's attacks ignore </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>200</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;(+25)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DEF when attacking enemies blocked by the Wolfpack and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.steal&gt;Steal&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{def_steal}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DEF from the target (Caps at </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{def_steal_max}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">After deployment, the next Operator has </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DP Cost. If the next Operator is a Melee Operator, gain </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DP</t>
-    </r>
-  </si>
-  <si>
-    <t>When Necrass or The Servant of Laments attack enemies with less than {%} HP, ATK + {}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can deploy up to 8 Rocky Chomper traps (Can store up to 10); The first enemy that steps on a trap will trigger its effect </t>
-  </si>
-  <si>
-    <t>Immediately puts up to &lt;@ba.vup&gt;{max_target}&lt;/&gt; enemies within Attack Range to &lt;$ba.sleep&gt;Sleep&lt;/&gt; and deal &lt;@ba.vup&gt;{atk_scale:0%}&lt;/&gt; ATK as Arts damage every &lt;@ba.vup&gt;{interval}&lt;/&gt; second. If the targets are defeated within the skill duration, summon &lt;@ba.vup&gt;{additional_token_cnt}&lt;/&gt; additional Servant of Laments</t>
-  </si>
-  <si>
-    <t>Passive: Each time The Servant of Lament is summoned or levelled up, deal &lt;@ba.vup&gt;{atk_scale:0%}&lt;/&gt; ATK as Arts damage to nearby enemies\n
-Active: Immediately resummon all Servant of Laments. If there are no Servant of Laments currently on the field, summon 1 Servant of Laments instead</t>
-  </si>
-  <si>
-    <t>When an enemy within Attack Range is defeated, summon The Servant of Lament at its location (up to 3). If no more Servant of Laments can be summoned, upgrade one Servant of Lament instead (increase Block Count, HP, ATK and DEF)</t>
-  </si>
-  <si>
-    <t>Passive: Up to 1 Servant of Lament change into a special form which can only upgrade through skill up to a {attack@max_stack_cnt} times\n
-Active: Immediately deal @ba.vup&gt;{attack@atk_scale:0%}&lt;/&gt; ATK as Arts damage to all enemies within range, then consume 1 Servant of Lament to upgrade the special Servant and recover &lt;@ba.vup&gt;{attack@hp_ratio:0%}&lt;/&gt; HP (If The Servant of Lament is already levelled, this effect is doubled). After a The Servant of Lament is consumed, can repeat &lt;@ba.vup&gt;{attack@necras_s_3[attack_cnt].max_stack_cnt}&lt;/&gt; times</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Passive Effect: When a trap is triggered, deals </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{atk_scale:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Physical damage to all enemies in range and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.stun&gt;stun&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> them for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;{stun}&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> second(s)\nActive Effect: Immediately gets 1 trap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Passive Effect: When a trap is triggered, deals </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{atk_scale:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Physical damage &lt;@ba.vup&gt;twice&lt;/&gt; to all enemies in range and inflicts </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-{-def:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DEF (does not stack) to the targets for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{duration}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds\nActive Effect: Immediately gets 1 trap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The next attack deals </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{attack@atk_scale:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Physical damage, and repeatedly bounce between enemies (up to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;{times}&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> times)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ATK </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+{atk:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, projectiles stick on target </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.sluggish&gt;slow&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> them for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;{attack@sluggish}&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds and slash them for &lt;@ba.vup&gt;4&lt;/&gt; additional times</t>
-    </r>
-  </si>
-  <si>
-    <t>When there are elite or leader enemies within Attack Range, increase SP recovery rate by +0.25 SP/sec</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cannot block enemies but gain </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.camou&gt;camouflage&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> during the skill duration</t>
-    </r>
+      <t>&lt;@ba.vup&gt;+{attack@chain.extra_value}&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Can summon a Reconstruct on a ground tile within Attack Range and can only be healed by Mon3tr. Allies around the Reconstruct ATK + {}. When the Reconstruct receives heals from itself or Mon3tr, bounces addition heal with same healing amount</t>
+  </si>
+  <si>
+    <t>When Mon3tr or the Reconstruct heals a target, self and the target's ASPD + {} for {} seconds (does not stack)</t>
+  </si>
+  <si>
+    <t>Prioritize healing the Reconstruct during skill. The Reconstruct also perform a bouncing heal when healed by Mon3tr. Increase the effect of the seconds talent to {}x</t>
+  </si>
+  <si>
+    <t>Attack Range change, &lt;$ba.addash&gt;move&lt;/&gt; to the Reconstruct position, ATK + {}, reduce Attack Interval {}, block count + {}, Max HP + {}, gradually lose {} HP, attacks all blocked enemies as True damage. Attacks recover HP by {} ATK. &lt;@ba.rem&gt;When skill ends or defeated, returns to original position.&lt;/&gt;</t>
   </si>
 </sst>
 </file>
@@ -3265,7 +3082,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3331,9 +3148,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3375,9 +3190,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4412,9 +4224,9 @@
   <colors>
     <mruColors>
       <color rgb="FF0098FF"/>
+      <color rgb="FFF49800"/>
       <color rgb="FF00B0FF"/>
       <color rgb="FFFF6237"/>
-      <color rgb="FFF49800"/>
     </mruColors>
   </colors>
   <extLst>
@@ -4455,8 +4267,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{89FBA152-941F-4C6C-9390-9532CA4293BB}" name="Table3" displayName="Table3" ref="A1:C9" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
-  <autoFilter ref="A1:C9" xr:uid="{7164C410-742E-4DED-83AD-C968A0703731}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{89FBA152-941F-4C6C-9390-9532CA4293BB}" name="Table3" displayName="Table3" ref="A1:C10" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+  <autoFilter ref="A1:C10" xr:uid="{7164C410-742E-4DED-83AD-C968A0703731}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{02CB2482-4BEC-4C01-B0C0-4F5BA3430F91}" name="Op" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{2BC33E28-91E4-4508-BBCC-48E211CE6FDE}" name="Skill" dataDxfId="17"/>
@@ -4467,8 +4279,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B14CCD12-F052-42BB-91EE-735614455405}" name="Table4" displayName="Table4" ref="A1:C23" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:C23" xr:uid="{8B5B2D93-E296-4982-9188-1B1EA292AE95}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B14CCD12-F052-42BB-91EE-735614455405}" name="Table4" displayName="Table4" ref="A1:C29" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:C29" xr:uid="{8B5B2D93-E296-4982-9188-1B1EA292AE95}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C9">
     <sortCondition ref="A2:A9"/>
     <sortCondition ref="B2:B9"/>
@@ -4483,8 +4295,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BCADEFEA-1805-4979-9482-D8E3D6498FC3}" name="Table5" displayName="Table5" ref="A1:D4" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D4" xr:uid="{3AD9D22D-2502-4D5C-8AA0-534854093817}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BCADEFEA-1805-4979-9482-D8E3D6498FC3}" name="Table5" displayName="Table5" ref="A1:D3" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D3" xr:uid="{3AD9D22D-2502-4D5C-8AA0-534854093817}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7324A2AE-1F85-4F21-8A09-2886AAE0CF24}" name="New" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{A602D952-3063-4C60-8090-59FB6704A6C8}" name="From" dataDxfId="2"/>
@@ -4761,8 +4573,8 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4796,7 +4608,7 @@
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -4813,7 +4625,7 @@
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -4830,7 +4642,7 @@
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -4847,7 +4659,7 @@
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -4864,7 +4676,7 @@
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -4881,7 +4693,7 @@
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="37" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -4898,7 +4710,7 @@
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -4915,7 +4727,7 @@
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="37" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -4932,7 +4744,7 @@
       <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="37" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -4949,7 +4761,7 @@
       <c r="A11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -4966,7 +4778,7 @@
       <c r="A12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -4983,7 +4795,7 @@
       <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -5000,7 +4812,7 @@
       <c r="A14" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="37" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -5017,7 +4829,7 @@
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -5034,7 +4846,7 @@
       <c r="A16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="37" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -5051,7 +4863,7 @@
       <c r="A17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="37" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -5068,7 +4880,7 @@
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="37" t="s">
         <v>55</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -5085,7 +4897,7 @@
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="37" t="s">
         <v>58</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -5102,7 +4914,7 @@
       <c r="A20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="37" t="s">
         <v>61</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -5119,7 +4931,7 @@
       <c r="A21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="37" t="s">
         <v>64</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -5136,7 +4948,7 @@
       <c r="A22" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="37" t="s">
         <v>67</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -5153,7 +4965,7 @@
       <c r="A23" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="37" t="s">
         <v>69</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -5170,7 +4982,7 @@
       <c r="A24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="37" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -5187,7 +4999,7 @@
       <c r="A25" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="37" t="s">
         <v>75</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -5204,7 +5016,7 @@
       <c r="A26" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="37" t="s">
         <v>78</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -5221,7 +5033,7 @@
       <c r="A27" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="37" t="s">
         <v>81</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -5238,7 +5050,7 @@
       <c r="A28" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="37" t="s">
         <v>84</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -5255,7 +5067,7 @@
       <c r="A29" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="37" t="s">
         <v>87</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -5272,7 +5084,7 @@
       <c r="A30" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="37" t="s">
         <v>90</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -5289,7 +5101,7 @@
       <c r="A31" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="37" t="s">
         <v>93</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -5306,7 +5118,7 @@
       <c r="A32" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="37" t="s">
         <v>96</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -5323,7 +5135,7 @@
       <c r="A33" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="37" t="s">
         <v>99</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -5340,7 +5152,7 @@
       <c r="A34" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="37" t="s">
         <v>102</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -5357,7 +5169,7 @@
       <c r="A35" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="37" t="s">
         <v>105</v>
       </c>
       <c r="C35" s="7" t="s">
@@ -5374,7 +5186,7 @@
       <c r="A36" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="37" t="s">
         <v>108</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -5391,7 +5203,7 @@
       <c r="A37" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="37" t="s">
         <v>111</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -5408,7 +5220,7 @@
       <c r="A38" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="37" t="s">
         <v>114</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -5425,7 +5237,7 @@
       <c r="A39" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="37" t="s">
         <v>117</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -5442,7 +5254,7 @@
       <c r="A40" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="37" t="s">
         <v>120</v>
       </c>
       <c r="C40" s="7" t="s">
@@ -5459,7 +5271,7 @@
       <c r="A41" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="37" t="s">
         <v>123</v>
       </c>
       <c r="C41" s="7" t="s">
@@ -5476,7 +5288,7 @@
       <c r="A42" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="37" t="s">
         <v>126</v>
       </c>
       <c r="C42" s="7" t="s">
@@ -5493,7 +5305,7 @@
       <c r="A43" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="37" t="s">
         <v>129</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -5510,7 +5322,7 @@
       <c r="A44" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="37" t="s">
         <v>132</v>
       </c>
       <c r="C44" s="7" t="s">
@@ -5527,7 +5339,7 @@
       <c r="A45" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="37" t="s">
         <v>135</v>
       </c>
       <c r="C45" s="7" t="s">
@@ -5544,7 +5356,7 @@
       <c r="A46" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B46" s="39" t="s">
+      <c r="B46" s="37" t="s">
         <v>138</v>
       </c>
       <c r="C46" s="7" t="s">
@@ -5561,7 +5373,7 @@
       <c r="A47" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="37" t="s">
         <v>140</v>
       </c>
       <c r="C47" s="7" t="s">
@@ -5578,7 +5390,7 @@
       <c r="A48" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="37" t="s">
         <v>142</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -5595,7 +5407,7 @@
       <c r="A49" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="37" t="s">
         <v>145</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -5612,7 +5424,7 @@
       <c r="A50" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="37" t="s">
         <v>148</v>
       </c>
       <c r="C50" s="7" t="s">
@@ -5629,7 +5441,7 @@
       <c r="A51" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B51" s="39" t="s">
+      <c r="B51" s="37" t="s">
         <v>153</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -5643,10 +5455,10 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="38" t="s">
         <v>206</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -5673,14 +5485,14 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.25" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="5"/>
-    <col min="3" max="3" width="203.875" style="35" customWidth="1"/>
+    <col min="3" max="3" width="203.875" style="33" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5691,7 +5503,7 @@
       <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5702,8 +5514,8 @@
       <c r="B2" s="18">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>241</v>
+      <c r="C2" s="31" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -5713,8 +5525,8 @@
       <c r="B3" s="18">
         <v>2</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>237</v>
+      <c r="C3" s="31" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -5724,8 +5536,8 @@
       <c r="B4" s="18">
         <v>1</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>238</v>
+      <c r="C4" s="31" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -5735,8 +5547,8 @@
       <c r="B5" s="18">
         <v>1</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>225</v>
+      <c r="C5" s="31" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -5750,17 +5562,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87E8A4C-DD19-471A-8655-5F20C6D67CEA}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
-    <col min="3" max="3" width="196.375" style="37" customWidth="1"/>
+    <col min="3" max="3" width="196.375" style="35" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5771,11 +5583,11 @@
       <c r="B1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>210</v>
       </c>
@@ -5783,10 +5595,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>210</v>
       </c>
@@ -5794,21 +5606,21 @@
         <v>2</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>210</v>
       </c>
       <c r="B4" s="21">
         <v>3</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C4" s="42" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>211</v>
       </c>
@@ -5816,10 +5628,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>211</v>
       </c>
@@ -5827,37 +5639,40 @@
         <v>2</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="40" t="s">
         <v>212</v>
       </c>
       <c r="B7" s="21">
         <v>1</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="40" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="41">
         <v>2</v>
       </c>
-      <c r="C8" s="45" t="s">
-        <v>246</v>
+      <c r="C8" s="42" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="s">
-        <v>226</v>
-      </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="43"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -5871,9 +5686,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F42A22B-36CC-4810-BF3A-03B3869F0BF4}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -5881,7 +5696,7 @@
   <cols>
     <col min="1" max="1" width="17.75" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
-    <col min="3" max="3" width="208.75" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="164.625" style="35" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5892,7 +5707,7 @@
       <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5903,35 +5718,41 @@
       <c r="B2" s="18">
         <v>2</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>228</v>
+      <c r="C2" s="31" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>213</v>
+      </c>
       <c r="B3" s="18">
         <v>2.5</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>229</v>
+      <c r="C3" s="31" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>213</v>
+      </c>
       <c r="B4" s="18">
         <v>3</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>228</v>
+      <c r="C4" s="31" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>213</v>
+      </c>
       <c r="B5" s="18">
         <v>3.5</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>229</v>
+      <c r="C5" s="31" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -5941,172 +5762,250 @@
       <c r="B6" s="18">
         <v>2</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>230</v>
+      <c r="C6" s="31" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>214</v>
+      </c>
       <c r="B7" s="18">
         <v>2.5</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>231</v>
+      <c r="C7" s="31" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>214</v>
+      </c>
       <c r="B8" s="18">
         <v>3</v>
       </c>
-      <c r="C8" s="33" t="s">
-        <v>230</v>
+      <c r="C8" s="31" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>214</v>
+      </c>
       <c r="B9" s="18">
         <v>3.5</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>231</v>
+      <c r="C9" s="31" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
-        <v>211</v>
+      <c r="A10" s="28" t="s">
+        <v>215</v>
       </c>
       <c r="B10" s="18">
         <v>2</v>
       </c>
-      <c r="C10" s="34" t="s">
-        <v>232</v>
+      <c r="C10" s="32" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="28" t="s">
+        <v>215</v>
+      </c>
       <c r="B11" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="18">
         <v>3</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="C12" s="32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="B12" s="18">
-        <v>2</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
       <c r="B13" s="18">
-        <v>3</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>233</v>
+        <v>3.5</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="28" t="s">
         <v>216</v>
       </c>
       <c r="B14" s="18">
         <v>2</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>234</v>
+      <c r="C14" s="32" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="28" t="s">
+        <v>216</v>
+      </c>
       <c r="B15" s="18">
         <v>2.5</v>
       </c>
-      <c r="C15" s="33" t="s">
-        <v>235</v>
+      <c r="C15" s="32" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
+      <c r="A16" s="28" t="s">
+        <v>216</v>
+      </c>
       <c r="B16" s="18">
         <v>3</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>234</v>
+      <c r="C16" s="32" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
+      <c r="A17" s="28" t="s">
+        <v>216</v>
+      </c>
       <c r="B17" s="18">
         <v>3.5</v>
       </c>
-      <c r="C17" s="33" t="s">
-        <v>235</v>
+      <c r="C17" s="32" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="28" t="s">
         <v>217</v>
       </c>
       <c r="B18" s="18">
         <v>2</v>
       </c>
-      <c r="C18" s="34" t="s">
-        <v>236</v>
+      <c r="C18" s="32" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
+      <c r="A19" s="7" t="s">
+        <v>217</v>
+      </c>
       <c r="B19" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" s="18">
         <v>3</v>
       </c>
-      <c r="C19" s="34" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="30" t="s">
+      <c r="C20" s="32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B21" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B22" s="18">
         <v>2</v>
       </c>
-      <c r="C20" s="34" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="30"/>
-      <c r="B21" s="18">
+      <c r="C22" s="32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" s="18">
+        <v>3</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="18">
+        <v>2</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" s="18">
         <v>2.5</v>
       </c>
-      <c r="C21" s="30" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="18">
+      <c r="C25" s="31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="18">
         <v>3</v>
       </c>
-      <c r="C22" s="34" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="18">
+      <c r="C26" s="31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" s="18">
         <v>3.5</v>
       </c>
-      <c r="C23" s="30" t="s">
-        <v>220</v>
-      </c>
+      <c r="C27" s="31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="32"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="7"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6119,10 +6018,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA072BA0-A74B-4D64-9677-E60E9F767C6E}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6135,54 +6034,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="26" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>224</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>227</v>
+      <c r="A2" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="24" t="s">
-        <v>247</v>
-      </c>
+      <c r="A3" s="43"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[CN] Fantasy in The Mirage
</commit_message>
<xml_diff>
--- a/temp/temp.xlsx
+++ b/temp/temp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AN-EN-Tags-NEW\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AN-EN-Tags\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE47A0F7-25B7-4FE7-B7BA-B0AEC575D252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEEBBB0-3331-415E-9424-0991D111C01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="645" windowWidth="21600" windowHeight="14835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KW" sheetId="5" r:id="rId1"/>
@@ -19,17 +19,26 @@
     <sheet name="Mod" sheetId="3" r:id="rId4"/>
     <sheet name="Trait" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="250">
   <si>
     <t>Op</t>
   </si>
@@ -1827,7 +1836,404 @@
     <t>Explodes when at max (1000 for Normal and Elite, 2000 for Leaders), dealing 6000 Elemental Damage and inflict 3 &lt;$ba.palsy&gt;Paralysis&lt;/&gt; stack. 10s cooldown.</t>
   </si>
   <si>
-    <t>Miss Christine</t>
+    <r>
+      <t>&lt;$ba.dt.element&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Elemental Injury</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Lure / Attract</t>
+  </si>
+  <si>
+    <t>Mod Trait</t>
+  </si>
+  <si>
+    <t>Cannot be blocked and move to target position.</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;$ba.attract&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Attract</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>ba.attract</t>
+  </si>
+  <si>
+    <t>Record Keeper</t>
+  </si>
+  <si>
+    <t>Leizi the Thunderbringer</t>
+  </si>
+  <si>
+    <t>Typhon</t>
+  </si>
+  <si>
+    <t>Heavy as the Swamp's Mire</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Goldenglow</t>
+  </si>
+  <si>
+    <t>Precise Redirection</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Goldenglow and her Drones' attacks ignore </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> RES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Goldenglow and her Drones' attacks ignore </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;(+3)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> RES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When damaging an enemy for the first and the second times while a skill is active, ATK increases to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.sluggish&gt;Slows&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> targets for 3 seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When damaging an enemy for the first and the second times while a skill is active, ATK increases to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;(+10%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.sluggish&gt;Slows&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> targets for 3 seconds</t>
+    </r>
+  </si>
+  <si>
+    <t>Gavial the Invincible</t>
+  </si>
+  <si>
+    <t>Medical Background</t>
+  </si>
+  <si>
+    <t>SIE-Y</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The further away the enemy, the higher the damage dealt (up to an increase of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;{damage_scale:0%}&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Details </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Details </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Increases the heal amount of the next heal to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;{heal_scale:0%}&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK and heal one additional target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF49800"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;@ba.rem&gt;Can store </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF49800"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> charges&lt;/&gt;</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1836,12 +2242,702 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;+{atk:0%}&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, when healing target, cause target to recover </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HP whenever taking damage for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>When an operator in Attack Range activate skill, recover 1 SP and ASPD+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Each tile within Attack Range has </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% chance to Lightning strikes every second, deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Arts damage to all enemies; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.fly&gt;Take Off&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when skill is inactive. When skill is active, increase ATK to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When skill is activated, Lightning strikes all ground tile within Attack Range, deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% ATK as Arts damage to ground enemies and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.tremble&gt;frighten&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> them for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Attack Range </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;expand&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on frontal and side direction. Deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>% ATK as Physical damage to ground enemies in all three direction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;@ba.rem&gt;Can store </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> charges; Trait effect will not reset until all skill charges depleted&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Attack Range </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;expand&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> along ground tiles up to 3 tiles. Attack deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>% ATK as Physical damage. ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> each time Lightning strikes during skill (up to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> stacks)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Attack Range </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;expand&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Attack Interval is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF49800"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;@ba.vdown&gt;greatly increased&lt;/&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Attack deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% ATK as Physical damage and generate electric currents on target in all direction, currents travel for 3 tiles. When current hit Leizi or high ground, current rebound, deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% ATK as Arts damage to enemies in currents tile every 0.6 seconds and has </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% chance to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.tremble&gt;frighten&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> them for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enemies blocked by this unit receive </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% Physical Fragility; Increases this unit's healing received by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">%, increased to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>% when under half HP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enemies blocked by this unit receive </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% Physical Fragility; Increases this unit's healing received by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FF00B0FF"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.vup&gt;+</t>
+      <t>&lt;@ba.talpu&gt;(+5%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, increased to </t>
     </r>
     <r>
       <rPr>
@@ -1851,17 +2947,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>{atk:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/&gt;, attacks deal an additional </t>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% </t>
     </r>
     <r>
       <rPr>
@@ -1871,1884 +2967,25 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{attack@ep_damage_ratio:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of Arts damage as </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Enemies within Attack Range take </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Elemental Damage when they </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.palsy&gt;Paralyze&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Stop attacking. Summon cat spirit at target location, deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Arts damage to neaby enemies every second; if target is under the burst effect of </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, deal an additional </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;{attack@extra_ep_damage_scale:0%}&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Elemental Damage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If this unit hasn't attacked for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds, dodge next attack.</t>
-    </r>
-  </si>
-  <si>
-    <t>Tippi</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.liftoff&gt;Takes Off&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, Attack Range </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;expands&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, ATK </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{atk:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.liftoff&gt;Takes Off&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, Attack Range </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;expands&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, ATK </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{atk:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, Shoots </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{times}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> times in a row; Only activated when attacked and dodge that attack</t>
-    </r>
-  </si>
-  <si>
-    <t>Tragodia</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Attacks deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Additionally, deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to enemies near target.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Enemies under the burst effect of </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, ASPD </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{-}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">; Enemies within Attack Range receive </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> when attacking</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;$ba.dt.element&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Elemental Injury</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{atk_scale:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Arts damage twice and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.root&gt;bind&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> enemy for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds. While Bound, the target takes </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> more </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, prioritizing enemies not under a burst effect</t>
-    </r>
-  </si>
-  <si>
-    <t>Lure / Attract</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Attack Range </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;expands&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, ATK </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{atk:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and prioritizing enemies not under a burst effect. Enemies that have received </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from Tragodia will receive </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Neural Impairment every second until Elemental burst; Enemies within Attack Range recover from burst effect of </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> faster. Whenever a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> burst effect is triggered, summon/refresh the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cage of Madness</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> at target location</t>
-    </r>
-  </si>
-  <si>
-    <t>Necrass</t>
-  </si>
-  <si>
-    <t>2+</t>
-  </si>
-  <si>
-    <t>3+</t>
-  </si>
-  <si>
-    <t>Tecno</t>
-  </si>
-  <si>
-    <t>Mod Trait</t>
-  </si>
-  <si>
-    <t>Techno</t>
-  </si>
-  <si>
-    <t>When a ground enemy within Attack Range is defeated, create a stronger Puppet Dancer at its location (up to 5). Puppet Dancers deal Arts damage</t>
-  </si>
-  <si>
-    <t>Ascalon</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Attacks inflict the following effect on enemies: Movement Speed reduced by 18% and take 10% of Ascalon's current ATK as Arts damage per second for 25s, stacking up to 3 times. Recover </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> HP whenever an enemy is defeated while this effect is active.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>When an enemy within Attack Range is defeated, ATK +</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds and summon The Servant of Lament at its location (up to 3). If no more Servant of Laments can be summoned, upgrade 1 Servant of Lament instead (increase Block Count, higher HP, higher ATK and higher DEF) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>When a ground enemy within Attack Range is defeated, create a stronger Puppet Dancer at its location (up to 5). Puppet Dancers deal Arts damage. While a Puppet is present, ATK +</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>When an enemy within Attack Range is defeated, self and summons ATK +</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds and summon The Servant of Lament at its location (up to 3). If no more Servant of Laments can be summoned, upgrade 1 Servant of Lament instead (increase Block Count, higher HP, higher ATK and higher DEF) </t>
-    </r>
-  </si>
-  <si>
-    <t>Dorothy</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Can deploy up to 8 Resonators (Can store up to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">); The first enemy that steps on a Resonator will trigger its effect. On deployment, immediately deploys </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Resonators within Attack Range </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Can deploy up to 10 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;(+2)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Resonators (Can store up to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">); The first enemy that steps on a Resonator will trigger its effect. On deployment, immediately deploys </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Resonators within Attack Range</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Can deploy up to 10 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;(+2)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Resonators (Can store up to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">); The first enemy that steps on a Resonator will trigger its effect. On deployment, immediately deploys </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Resonators within Attack Range; Has </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> chance to deploy an additional trap in Attack Range when deploying a trap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Can deploy up to 8 Resonators (Can store up to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">); The first enemy that steps on a Resonator will trigger its effect. On deployment, immediately deploys </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Resonators within Attack Range; Has </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> chance to deploy an additional trap in Attack Range when deploying a trap</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Can deploy </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> additional trap and trap deployment costs are reduced</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Attack Range </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;expands&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Check CN text)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Can attack enemy blocked by own summon; ATK is increased to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{atk_scale:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> when attacking enemies blocked by own summon</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Elemental Injury dealt to Elite and Leader enemies increases by </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>18%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Check CN text)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Deals Damage to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;all targets&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> within range\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>65%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> chance to dodge Physical and Arts attacks and is less likely to be </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;targeted&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> by enemies </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Check CN text)</t>
-    </r>
-  </si>
-  <si>
-    <t>Mountain</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">DEF +10%; Physical Dodge +15%; When dodge an attack, next attack </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.tremble&gt;Frighten&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> target for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ASPD </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{aspd:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, splash area effect of the first talent increased; Can summon </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Blood's whisper</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, the summon </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attact</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> enemies in for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds (prioritize elite and leader enemies). After target reach the summon, retreat the summon, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.sluggish&gt;slow&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> nearby enemies for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds, deal both </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{atk_scale:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Arts damage and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{attack@ep_damage_ratio:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.dt.neural2&gt;Nervous Impairment&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> every 0.5 seconds; Catto has its own redeployment time </t>
-    </r>
-  </si>
-  <si>
-    <t>Cannot be blocked and move to target position.</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;$ba.attract&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Attract</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>ba.attract</t>
+      <t>&lt;@ba.talpu&gt;(+5%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when under half HP</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3800,6 +3037,20 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3953,7 +3204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4063,11 +3314,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="38">
     <dxf>
       <font>
         <b val="0"/>
@@ -4322,6 +3577,34 @@
         <bottom style="thin">
           <color theme="0" tint="-0.499984740745262"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -5069,8 +4352,8 @@
   <colors>
     <mruColors>
       <color rgb="FF0098FF"/>
+      <color rgb="FFF49800"/>
       <color rgb="FF00B0FF"/>
-      <color rgb="FFF49800"/>
       <color rgb="FFFF6237"/>
     </mruColors>
   </colors>
@@ -5086,53 +4369,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C16CB9E1-C747-45DF-B3A2-348B6D400693}" name="Table1" displayName="Table1" ref="A1:E52" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C16CB9E1-C747-45DF-B3A2-348B6D400693}" name="Table1" displayName="Table1" ref="A1:E52" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34">
   <autoFilter ref="A1:E52" xr:uid="{373BD71A-3DF4-4BC2-B1FE-B89A538D34FF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1BDC0A72-6D09-4EE6-A806-0E6B91CABBAA}" name="Keyword" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{07C2DF2B-28B9-440F-BAE8-1CBC9A743A7E}" name="Type" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{C0AE2D09-B9F4-4996-A1F9-3C21AB7EDA04}" name="kw" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{2D825A5B-8764-4E3E-8043-70A50DB4AB22}" name="Color" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{7C465D26-20BE-4736-A643-089B09CA7FD8}" name="Details" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{1BDC0A72-6D09-4EE6-A806-0E6B91CABBAA}" name="Keyword" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{07C2DF2B-28B9-440F-BAE8-1CBC9A743A7E}" name="Type" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{C0AE2D09-B9F4-4996-A1F9-3C21AB7EDA04}" name="kw" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{2D825A5B-8764-4E3E-8043-70A50DB4AB22}" name="Color" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{7C465D26-20BE-4736-A643-089B09CA7FD8}" name="Details" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6968D02B-2C35-4522-99E1-BA51530B4553}" name="Table2" displayName="Table2" ref="A1:C9" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6968D02B-2C35-4522-99E1-BA51530B4553}" name="Table2" displayName="Table2" ref="A1:C9" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:C9" xr:uid="{71236087-20BC-4953-BFDF-0CA4834863A9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D84A1065-D5C9-46A0-A7AB-4B9ADC68B4C5}" name="Op" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{38256F81-A768-4F88-935E-457B88738A34}" name="Talent" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{54030400-8D62-49B2-BCCF-83684F84DEAA}" name="Details" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{D84A1065-D5C9-46A0-A7AB-4B9ADC68B4C5}" name="Op" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{38256F81-A768-4F88-935E-457B88738A34}" name="Talent" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{54030400-8D62-49B2-BCCF-83684F84DEAA}" name="Details &lt;@ba.talpu&gt;{}&lt;/&gt;" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{89FBA152-941F-4C6C-9390-9532CA4293BB}" name="Table3" displayName="Table3" ref="A1:C12" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{89FBA152-941F-4C6C-9390-9532CA4293BB}" name="Table3" displayName="Table3" ref="A1:C12" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="A1:C12" xr:uid="{7164C410-742E-4DED-83AD-C968A0703731}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{02CB2482-4BEC-4C01-B0C0-4F5BA3430F91}" name="Op" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{2BC33E28-91E4-4508-BBCC-48E211CE6FDE}" name="Skill" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{212359CB-4A30-4872-99A6-07552DAAAE97}" name="Details" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{02CB2482-4BEC-4C01-B0C0-4F5BA3430F91}" name="Op" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{2BC33E28-91E4-4508-BBCC-48E211CE6FDE}" name="Skill" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{212359CB-4A30-4872-99A6-07552DAAAE97}" name="Details " dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B14CCD12-F052-42BB-91EE-735614455405}" name="Table4" displayName="Table4" ref="A1:C17" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:C17" xr:uid="{8B5B2D93-E296-4982-9188-1B1EA292AE95}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B14CCD12-F052-42BB-91EE-735614455405}" name="Table4" displayName="Table4" ref="A1:D17" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A1:D17" xr:uid="{8B5B2D93-E296-4982-9188-1B1EA292AE95}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D8">
     <sortCondition ref="A2:A8"/>
     <sortCondition ref="B2:B8"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{230E321A-FD9D-4A88-BDB2-D4521C6A9226}" name="Op" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{F0081EE5-F0F2-4F94-AA73-769EF87E7EB6}" name="Level" dataDxfId="9"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{230E321A-FD9D-4A88-BDB2-D4521C6A9226}" name="Op" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{F0081EE5-F0F2-4F94-AA73-769EF87E7EB6}" name="Level" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{875AA631-11A6-427A-9BE7-3CC56886BA27}" name="Column1" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{224BD11C-823E-43C3-A2EF-F8A264F71916}" name="Detail" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5418,8 +4702,8 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5899,7 +5183,7 @@
         <v>202</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D28" s="14">
         <v>0</v>
@@ -6352,19 +5636,19 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>259</v>
+        <v>222</v>
       </c>
       <c r="B55" s="33" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>258</v>
+        <v>221</v>
       </c>
       <c r="D55" s="14">
         <v>0</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -6381,7 +5665,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6400,52 +5684,46 @@
         <v>7</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>1</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>225</v>
+      <c r="A2" s="41" t="s">
+        <v>224</v>
       </c>
       <c r="B2" s="18">
         <v>1</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>225</v>
+      <c r="A3" s="41" t="s">
+        <v>224</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B4" s="18">
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="B5" s="18">
-        <v>1</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>219</v>
-      </c>
+      <c r="A5" s="7"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
@@ -6480,15 +5758,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87E8A4C-DD19-471A-8655-5F20C6D67CEA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
-    <col min="3" max="3" width="196.375" style="31" customWidth="1"/>
+    <col min="3" max="3" width="255.625" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -6500,85 +5778,73 @@
         <v>2</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>225</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>224</v>
       </c>
       <c r="B2" s="18">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>225</v>
+      <c r="C2" s="42" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>224</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>225</v>
+      <c r="C3" s="42" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
+        <v>224</v>
       </c>
       <c r="B4" s="18">
         <v>3</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>231</v>
+      <c r="C4" s="21" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B5" s="18">
         <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B6" s="18">
         <v>2</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="B7" s="18">
-        <v>1</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="B8" s="38">
-        <v>2</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>220</v>
-      </c>
+      <c r="A7" s="7"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="36"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
@@ -6612,205 +5878,241 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F42A22B-36CC-4810-BF3A-03B3869F0BF4}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
-    <col min="3" max="3" width="164.625" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="164.625" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="27" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="27" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="27" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="27" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="B2" s="18">
-        <v>2</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B4" s="18">
-        <v>3</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="B6" s="18">
         <v>2</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C6" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="18">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="B7" s="18">
-        <v>3</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="18">
-        <v>2</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B9" s="18">
-        <v>3</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+        <v>3.5</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B10" s="18">
         <v>2</v>
       </c>
-      <c r="C10" s="28" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C10" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B11" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="18">
         <v>3</v>
       </c>
-      <c r="C11" s="28" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="B12" s="18">
+      <c r="C12" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" s="18">
         <v>2</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="B14" s="18">
+      <c r="C14" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="B16" s="18">
         <v>3</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C16" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" s="28" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="B15" s="18" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="B16" s="18">
-        <v>2</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>254</v>
-      </c>
       <c r="B17" s="18">
-        <v>3</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>255</v>
+        <v>3.5</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -6827,7 +6129,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6855,63 +6157,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="B2" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="39"/>
+      <c r="C2" s="39" t="s">
+        <v>236</v>
+      </c>
       <c r="D2" s="21" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
-        <v>236</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>232</v>
-      </c>
+      <c r="A3" s="39"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="24"/>
-      <c r="D3" s="30" t="s">
-        <v>251</v>
-      </c>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
-        <v>236</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>237</v>
-      </c>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="24"/>
-      <c r="D4" s="36" t="s">
-        <v>250</v>
-      </c>
+      <c r="D4" s="36"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>239</v>
-      </c>
+      <c r="A5" s="39"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="36" t="s">
-        <v>253</v>
-      </c>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
-        <v>236</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>244</v>
-      </c>
+      <c r="A6" s="39"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="39"/>
-      <c r="D6" s="21" t="s">
-        <v>249</v>
-      </c>
+      <c r="D6" s="21"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="37"/>

</xml_diff>

<commit_message>
[CN] IS#6 : Sui's Garden of Grotesqueries (RAW)
</commit_message>
<xml_diff>
--- a/temp/temp.xlsx
+++ b/temp/temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AN-EN-Tags\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEEBBB0-3331-415E-9424-0991D111C01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BB26D9-80A4-45E9-9071-A9F3E96AD79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="645" windowWidth="21600" windowHeight="14835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KW" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="238">
   <si>
     <t>Op</t>
   </si>
@@ -1898,29 +1898,46 @@
     <t>ba.attract</t>
   </si>
   <si>
-    <t>Record Keeper</t>
-  </si>
-  <si>
-    <t>Leizi the Thunderbringer</t>
-  </si>
-  <si>
-    <t>Typhon</t>
-  </si>
-  <si>
-    <t>Heavy as the Swamp's Mire</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
-    <t>Goldenglow</t>
-  </si>
-  <si>
-    <t>Precise Redirection</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Goldenglow and her Drones' attacks ignore </t>
+    <r>
+      <t xml:space="preserve">The further away the enemy, the higher the damage dealt (up to an increase of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;{damage_scale:0%}&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Details </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;</t>
     </r>
     <r>
       <rPr>
@@ -1935,17 +1952,39 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> RES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Goldenglow and her Drones' attacks ignore </t>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Details </t>
+  </si>
+  <si>
+    <t>Raidian</t>
+  </si>
+  <si>
+    <t>SO-A</t>
+  </si>
+  <si>
+    <t>summon</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;</t>
     </r>
     <r>
       <rPr>
@@ -1955,6 +1994,343 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>+{atk:0%}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/&gt; ATK and launch </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> additional shot</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Passive: Summons may be deployed on melee tiles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Active: Raidian and her summons gain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+{def:0%}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DEF and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.barrier&gt;Barrier&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> equal to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{hp_ratio:0%}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Max HP last until the skill ends
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.rem&gt;Immediately gain 1 summon when the skill is activated&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+{def:0%}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/&gt; DEF and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.barrier&gt;Barrier&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> equal to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;@ba.vup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{hp_ratio:0%}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Max HP last until the skill ends</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+{atk:0%}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/&gt; ATK, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.sluggish&gt;slow&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and inflict </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>{}</t>
     </r>
     <r>
@@ -1970,27 +2346,123 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.magicfragile&gt;Arts Fragility&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to target for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Can use up to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> summons (max </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> deployed at once). Summons’ effect changes based upon Skill </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Passive: Summons may be deployed on melee tiles and continuously launch a Straight Shot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Active: Raidian and her summons gain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FF00B0FF"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.talpu&gt;(+3)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> RES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When damaging an enemy for the first and the second times while a skill is active, ATK increases to </t>
+      <t>&lt;@ba.vup&gt;</t>
     </r>
     <r>
       <rPr>
@@ -2000,6 +2472,163 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>+{atk:0%}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK and summon launch </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> additional shot
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.rem&gt;Immediately gain 1 summon when the skill is activated&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Passive: Summons may be deployed on ranged tiles. When summon cannot find target in it own Attack Range, it can coordination attack with other summon in Attack Range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Active: Raidian and her summons gain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+{atk:0%}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK, summon </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.sluggish&gt;slow&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and inflict </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>{}</t>
     </r>
     <r>
@@ -2010,7 +2639,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">% and </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -2020,22 +2649,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;$ba.sluggish&gt;Slows&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> targets for 3 seconds</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When damaging an enemy for the first and the second times while a skill is active, ATK increases to </t>
+      <t>&lt;$ba.magicfragile&gt;Arts Fragility&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to target for </t>
     </r>
     <r>
       <rPr>
@@ -2055,144 +2679,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;(+10%)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.sluggish&gt;Slows&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> targets for 3 seconds</t>
-    </r>
-  </si>
-  <si>
-    <t>Gavial the Invincible</t>
-  </si>
-  <si>
-    <t>Medical Background</t>
-  </si>
-  <si>
-    <t>SIE-Y</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The further away the enemy, the higher the damage dealt (up to an increase of </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;{damage_scale:0%}&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Details </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Details </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Increases the heal amount of the next heal to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;{heal_scale:0%}&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK and heal one additional target</t>
+      <t xml:space="preserve"> seconds
+</t>
     </r>
     <r>
       <rPr>
@@ -2207,778 +2695,16 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFF49800"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;@ba.rem&gt;Can store </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF49800"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> charges&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ATK </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;+{atk:0%}&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, when healing target, cause target to recover </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> HP whenever taking damage for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>When an operator in Attack Range activate skill, recover 1 SP and ASPD+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Each tile within Attack Range has </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% chance to Lightning strikes every second, deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK as Arts damage to all enemies; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.fly&gt;Take Off&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> when skill is inactive. When skill is active, increase ATK to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>%.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When skill is activated, Lightning strikes all ground tile within Attack Range, deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% ATK as Arts damage to ground enemies and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.tremble&gt;frighten&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> them for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Attack Range </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;expand&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> on frontal and side direction. Deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>% ATK as Physical damage to ground enemies in all three direction</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
         <color rgb="FFFFC000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">&lt;@ba.rem&gt;Can store </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> charges; Trait effect will not reset until all skill charges depleted&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Attack Range </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;expand&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> along ground tiles up to 3 tiles. Attack deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>% ATK as Physical damage. ATK+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> each time Lightning strikes during skill (up to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> stacks)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Attack Range </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;expand&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, Attack Interval is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF49800"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;@ba.vdown&gt;greatly increased&lt;/&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Attack deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% ATK as Physical damage and generate electric currents on target in all direction, currents travel for 3 tiles. When current hit Leizi or high ground, current rebound, deal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% ATK as Arts damage to enemies in currents tile every 0.6 seconds and has </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% chance to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.tremble&gt;frighten&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> them for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Enemies blocked by this unit receive </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% Physical Fragility; Increases this unit's healing received by </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">%, increased to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>% when under half HP</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Enemies blocked by this unit receive </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% Physical Fragility; Increases this unit's healing received by </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;(+5%)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, increased to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.talpu&gt;(+5%)&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> when under half HP</t>
-    </r>
+      <t>&lt;@ba.rem&gt;Immediately gain 1 summon when the skill is activated&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Summons gain &lt;$ba.inspire&gt;Inspiration&lt;/&gt; equal to {} of Raidian's HP, ATK and DEF</t>
   </si>
 </sst>
 </file>
@@ -3204,7 +2930,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3317,7 +3043,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4352,8 +4077,8 @@
   <colors>
     <mruColors>
       <color rgb="FF0098FF"/>
+      <color rgb="FF00B0FF"/>
       <color rgb="FFF49800"/>
-      <color rgb="FF00B0FF"/>
       <color rgb="FFFF6237"/>
     </mruColors>
   </colors>
@@ -4702,8 +4427,8 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5665,7 +5390,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5684,41 +5409,35 @@
         <v>7</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B2" s="18">
         <v>1</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B4" s="18">
-        <v>1</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>242</v>
-      </c>
+      <c r="A4" s="7"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
@@ -5758,8 +5477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87E8A4C-DD19-471A-8655-5F20C6D67CEA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5778,68 +5497,68 @@
         <v>2</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B2" s="18">
         <v>1</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
       </c>
-      <c r="C3" s="42" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B4" s="18">
         <v>3</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B5" s="18">
-        <v>1</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="21" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B6" s="18">
-        <v>2</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="21" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>229</v>
+      </c>
       <c r="B7" s="18"/>
-      <c r="C7" s="21"/>
+      <c r="C7" s="21" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
@@ -5880,8 +5599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F42A22B-36CC-4810-BF3A-03B3869F0BF4}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5901,219 +5620,115 @@
         <v>3</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>224</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>227</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="7"/>
       <c r="D2" s="27" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>224</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>227</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="7"/>
       <c r="D3" s="27" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>223</v>
-      </c>
+      <c r="A4" s="7"/>
       <c r="B4" s="18"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="27" t="s">
-        <v>242</v>
-      </c>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>223</v>
-      </c>
+      <c r="A5" s="7"/>
       <c r="B5" s="18"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="27" t="s">
-        <v>242</v>
-      </c>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B6" s="18">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>232</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7" s="18">
-        <v>2.5</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>233</v>
-      </c>
+      <c r="A7" s="7"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B8" s="18">
-        <v>3</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>232</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B9" s="18">
-        <v>3.5</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>233</v>
-      </c>
+      <c r="A9" s="7"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="B10" s="18">
-        <v>2</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="A10" s="25"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="B11" s="18">
-        <v>2.5</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>231</v>
-      </c>
+      <c r="A11" s="25"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="28"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="B12" s="18">
-        <v>3</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="A12" s="25"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="B13" s="18">
-        <v>3.5</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>231</v>
-      </c>
+      <c r="A13" s="25"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="B14" s="18">
-        <v>2</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>248</v>
-      </c>
+      <c r="A14" s="25"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="28"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="B15" s="18">
-        <v>2.5</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>249</v>
-      </c>
+      <c r="A15" s="25"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="B16" s="18">
-        <v>3</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>248</v>
-      </c>
+      <c r="A16" s="25"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="B17" s="18">
-        <v>3.5</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>249</v>
-      </c>
+      <c r="A17" s="25"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6129,7 +5744,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6159,14 +5774,14 @@
       <c r="A2" s="39" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="39" t="s">
-        <v>225</v>
+      <c r="B2" s="41" t="s">
+        <v>227</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Special Operator : Unlock (exclude Proficiency)
</commit_message>
<xml_diff>
--- a/temp/temp.xlsx
+++ b/temp/temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AN-EN-Tags\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BB26D9-80A4-45E9-9071-A9F3E96AD79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720CADC3-CF24-42D0-9CB3-EC4FCF04CE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KW" sheetId="5" r:id="rId1"/>
@@ -5390,7 +5390,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5478,7 +5478,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5599,8 +5599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F42A22B-36CC-4810-BF3A-03B3869F0BF4}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5743,8 +5743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA072BA0-A74B-4D64-9677-E60E9F767C6E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Bandage : Skip talentless phase
</commit_message>
<xml_diff>
--- a/temp/temp.xlsx
+++ b/temp/temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AN-EN-Tags\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720CADC3-CF24-42D0-9CB3-EC4FCF04CE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF470A80-7E07-4FA2-91DD-596006B22568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KW" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="292">
   <si>
     <t>Op</t>
   </si>
@@ -1864,70 +1864,1334 @@
     <t>Lure / Attract</t>
   </si>
   <si>
+    <t>Cannot be blocked and move to target position.</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;$ba.attract&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Attract</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>ba.attract</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Details </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Details </t>
+  </si>
+  <si>
+    <t>Hoshiguma the Breacher</t>
+  </si>
+  <si>
+    <t>Haruka</t>
+  </si>
+  <si>
+    <t>Matsukiri</t>
+  </si>
+  <si>
+    <t>Trait</t>
+  </si>
+  <si>
+    <t>Strategist</t>
+  </si>
+  <si>
+    <t>Block 2 enemies\nCan support allies in the Deployment Waiting Zone</t>
+  </si>
+  <si>
+    <t>Kichisei</t>
+  </si>
+  <si>
+    <t>Nymph</t>
+  </si>
+  <si>
     <t>Mod Trait</t>
   </si>
   <si>
-    <t>Cannot be blocked and move to target position.</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;$ba.attract&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Attract</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
+    <t>Primal Caster</t>
+  </si>
+  <si>
+    <t>Increase damage dealt to enemies under elemental burst effect to 110%</t>
+  </si>
+  <si>
+    <t>Blaze the Igniting Spark</t>
+  </si>
+  <si>
+    <t>Diamante</t>
+  </si>
+  <si>
+    <t>Warmy</t>
+  </si>
+  <si>
+    <t>Miss.Christine</t>
+  </si>
+  <si>
+    <t>Ch'en the Holungday</t>
+  </si>
+  <si>
+    <t>Spreadshooter</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Gains 1 Coin upon skill activation (can be spent through skills). While a skill is active, gains 1 Coin each time DP is consumed by this unit's Trait, and +4% ATK (stacks up to 8 times)</t>
+  </si>
+  <si>
+    <t>Swire the Elegant Wit</t>
+  </si>
+  <si>
+    <t>Pepe</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When Bubble pop, Bubble operator recovery HP for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Increase damage for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for every unique enemy defeated (can stack </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Gains up to +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK and +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> RES </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.berserk&gt;Tenacity&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (reaches maximum bonus when losing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Max HP) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Every </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attack, grant </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.protect&gt;Sanctuary&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bubble to operator in Attack Range. When Bubble operator take damage, Bubble pop after </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Defender]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Supporter]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operators on the field and Deployment Waiting Zone ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> after Matsukiri has been deployed for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>When HP down to 0, enter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Self"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> state. During this period, cannot be healed by allies and accumulate all incoming damage. When accumulate damage higher than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Max HP, reteated. When not received any damage for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds, recover </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HP per seconds. When HP more than 0, exist </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Self"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> state.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ASPD+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. When Bubble pop, grant Bubble to all nearby operators in the surrounding 8 tiles.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hoshiguma throws her shield out, attack all blocked enemies and deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Arts damage thrice, shield spin around her once, deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Arts damage every 0.5 second and inflict </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.sluggish&gt;Slow&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to nearby enemies for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds; Hoshiguma recover HP by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of Shield damage dealt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Attack Range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;@ba.kw&gt;expand&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Max HP +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ATK +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, attack up to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> enemies twice. When deactivate skill manually, retain skill effect for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds and cannot be defeated. Attack deal damage four-in-a-row insteads, receive lethal damage dealt on other operators in Attack Range, automatically retreat after effect end.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.rem&gt;Skill can be manually deactivated&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Increase healing target and Bubble count by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. When operators healed by Haruka, deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of healing amount as Arts damage to enemies nearby.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.rem&gt;From second activation and on, ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, this skill has unlimited duration&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Attack Range </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;expand&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, attack interval </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;reduce&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Bubble </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.protect&gt;Sanctuary&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> effectiveness </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">x. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.levitate&gt;Levitate&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> enemies that attack Bubble operator for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds and deal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Arts damage every second to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.levitate&gt;Levitated&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> enemies.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Immediately gains </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{cost}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>&lt;/&gt;</t>
     </r>
-  </si>
-  <si>
-    <t>ba.attract</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The further away the enemy, the higher the damage dealt (up to an increase of </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.kw&gt;{damage_scale:0%}&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Details </t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{-}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DP cost of the right-most operator in Deployment Waiting Zone</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Attack interval </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF49800"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vdown&gt;increase slightly&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. After every attack, ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (can stack </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Attack interval </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF49800"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vdown&gt;increase&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Each attack randomly inflicts one of the following statuses to all targets hit (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.sluggish&gt;slow&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.root&gt;bind&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.stun&gt;stun&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) for </t>
     </r>
     <r>
       <rPr>
@@ -1937,7 +3201,82 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.talpu&gt;</t>
+      <t>&lt;@ba.vup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{sluggish}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gradually obtains </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.vup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{trig_cnt}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DP during the skill duration. While this skill is active, ATK+</t>
     </r>
     <r>
       <rPr>
@@ -1952,29 +3291,1159 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and recover </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HP every second. When skill end, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DP cost and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Max HP for all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Defender] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Supporter]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operators in Deployment Waiting Zone (can stack </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times until they retreated)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;Reduces&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Deployment Cost</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;Integrated Strategies&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, reduce deployment cost and on-field DP cost by 30%. For every DP consumed, reduce the Redeployment time of least remaining redeployment time operator by 2 seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;Reclamation Algorithm&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, when carry any resource, the Redeployment time greatly reduce</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When deployed, all </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Guard]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Operators gain +16% ATK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;Reclamation Algorithm&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, reveal Treasure chest location, attack create shockwave on all other </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Guard]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operators</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;Reclamation Algorithm&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, reveal Treasure chest location, attack create 50% ATK shockwave on all other </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Guard]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operators. When has resource as Primary target create 50% ATK shockwave on all connected resources (up to 10 resources)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When Bubble pop, Bubble operator recovery HP for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK and has </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chance to recover 1 SP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Whenever a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.apoptosis2&gt;Necrosis damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst effect is triggered, ATK +2%, stacking up to 10 times. After 10 stack, ASPD+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Whenever a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.apoptosis2&gt;Necrosis damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst effect is triggered, ATK +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%, stacking up to 10 times. After 10 stack, ASPD+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Whenever an enemy triggers a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.burning2&gt;Burn damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst, immediately deals </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>% ATK as Elemental Damage to that enemy, recovers 12% Max HP and ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Whenever an enemy triggers a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.burning2&gt;Burn damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst, immediately deals </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% ATK as Elemental Damage to that enemy, recovers </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>% Max HP and ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If there is an enemy within attack range under the burst effect of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.apoptosis2&gt;Necrosis damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ATK +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enemies within Attack Range take </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% ATK as Elemental Damage when they trigger a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.burning2&gt;Burn damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When attack </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.palsy&gt;Paralyze&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> enemies, increase ATK to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Enemies within Attack Range take </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% ATK as Elemental Damage when they </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.palsy&gt;Paralyze&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ASPD +8, when there is water terrain on the battlefield, the effect becomes ASPD +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ASPD +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, when there is water terrain on the battlefield, the effect becomes ASPD +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. When skill is active, regard the battlefield as water terrain</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;Integrated Strategies&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Coin limit +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, gains 1 extra Coin each time DP is consumed by this unit's Trait and gain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> additional ATK stack</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.kw&gt;Integrated Strategies&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Coin limit +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, maximum ATK stack +1 for each Originium Ingot in possession (up to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> additional max stacks), gains 1 extra Coin each time DP is consumed by this unit's Trait and gain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> additional ATK stack</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Whenever a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.apoptosis2&gt;Necrosis damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst effect is triggered, ATK +2%, stacking up to 12 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FF00B0FF"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Details </t>
-  </si>
-  <si>
-    <t>Raidian</t>
-  </si>
-  <si>
-    <t>SO-A</t>
-  </si>
-  <si>
-    <t>summon</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Gain </t>
+      <t>&lt;@ba.talpu&gt;(+2)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times. After 10 stack, ASPD+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Whenever a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.apoptosis2&gt;Necrosis damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst effect is triggered, ATK +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">%, stacking up to 12 </t>
     </r>
     <r>
       <rPr>
@@ -1984,73 +4453,72 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+{atk:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/&gt; ATK and launch </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> additional shot</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Passive: Summons may be deployed on melee tiles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Active: Raidian and her summons gain </t>
+      <t>&lt;@ba.talpu&gt;(+2)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times. After 10 stack, ASPD+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Whenever an enemy triggers a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.burning2&gt;Burn damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst, immediately deals </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% </t>
     </r>
     <r>
       <rPr>
@@ -2060,17 +4528,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+{def:0%}</t>
+      <t>&lt;@ba.talpu&gt;(+30%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Elemental Damage to that enemy, recovers 15% </t>
     </r>
     <r>
       <rPr>
@@ -2080,37 +4548,102 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DEF and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.barrier&gt;Barrier&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> equal to </t>
+      <t>&lt;@ba.talpu&gt;(+3%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Max HP and ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Whenever an enemy triggers a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.burning2&gt;Burn damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst, immediately deals </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% </t>
     </r>
     <r>
       <rPr>
@@ -2120,17 +4653,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{hp_ratio:0%}</t>
+      <t>&lt;@ba.talpu&gt;(+30%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Elemental Damage to that enemy, recovers </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% </t>
     </r>
     <r>
       <rPr>
@@ -2140,43 +4693,102 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Max HP last until the skill ends
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.rem&gt;Immediately gain 1 summon when the skill is activated&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Gain </t>
+      <t>&lt;@ba.talpu&gt;(+3%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Max HP and ATK+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> seconds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If there is an enemy within attack range under the burst effect of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.apoptosis2&gt;Necrosis damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ATK +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">% </t>
     </r>
     <r>
       <rPr>
@@ -2186,47 +4798,32 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+{def:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/&gt; DEF and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.barrier&gt;Barrier&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> equal to</t>
+      <t>&lt;@ba.talpu&gt;(+3%)&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enemies within Attack Range take </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%</t>
     </r>
     <r>
       <rPr>
@@ -2236,17 +4833,102 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> &lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{hp_ratio:0%}</t>
+      <t>&lt;@ba.talpu&gt; (+20%) &lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ATK as Elemental Damage when they trigger a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.dt.burning2&gt;Burn damage&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> burst</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When attack </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.palsy&gt;Paralyze&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> enemies, increase ATK to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Enemies within Attack Range take </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%</t>
     </r>
     <r>
       <rPr>
@@ -2256,22 +4938,32 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Max HP last until the skill ends</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Gain </t>
+      <t>&lt;@ba.talpu&gt;(+10%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Elemental Damage when they </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;$ba.palsy&gt;Paralyze&lt;/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gains 1 Coin upon skill activation (can be spent through skills). While a skill is active, gains 1 Coin each time DP is consumed by this unit's Trait, and +4% ATK (stacks up to 9 </t>
     </r>
     <r>
       <rPr>
@@ -2281,47 +4973,67 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+{atk:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/&gt; ATK, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.sluggish&gt;slow&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and inflict </t>
+      <t>&lt;@ba.talpu&gt;(+1)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When deployed, all </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0098FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Guard]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Operators gain +20% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0FF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;@ba.talpu&gt;(+4%)&lt;/&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ATK+</t>
     </r>
     <r>
       <rPr>
@@ -2341,27 +5053,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.magicfragile&gt;Arts Fragility&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to target for </t>
+      <t>, DEF+</t>
     </r>
     <r>
       <rPr>
@@ -2381,330 +5073,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> seconds</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Can use up to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> summons (max </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> deployed at once). Summons’ effect changes based upon Skill </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Passive: Summons may be deployed on melee tiles and continuously launch a Straight Shot</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Active: Raidian and her summons gain </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+{atk:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK and summon launch </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> additional shot
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.rem&gt;Immediately gain 1 summon when the skill is activated&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Passive: Summons may be deployed on ranged tiles. When summon cannot find target in it own Attack Range, it can coordination attack with other summon in Attack Range</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Active: Raidian and her summons gain </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.vup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+{atk:0%}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ATK, summon </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.sluggish&gt;slow&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and inflict </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0098FF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;$ba.magicfragile&gt;Arts Fragility&lt;/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to target for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> seconds
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;@ba.rem&gt;Immediately gain 1 summon when the skill is activated&lt;/&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>Summons gain &lt;$ba.inspire&gt;Inspiration&lt;/&gt; equal to {} of Raidian's HP, ATK and DEF</t>
+      <t>. Deals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ATK as Arts damage to enemies that attack Hoshiguma\n&lt;@ba.rem&gt;From second activation and on, ATK+{}, this skill has unlimited duration&lt;/&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2930,7 +5320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3043,6 +5433,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4076,8 +6467,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00B0FF"/>
       <color rgb="FF0098FF"/>
-      <color rgb="FF00B0FF"/>
       <color rgb="FFF49800"/>
       <color rgb="FFFF6237"/>
     </mruColors>
@@ -4132,8 +6523,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B14CCD12-F052-42BB-91EE-735614455405}" name="Table4" displayName="Table4" ref="A1:D17" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
-  <autoFilter ref="A1:D17" xr:uid="{8B5B2D93-E296-4982-9188-1B1EA292AE95}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B14CCD12-F052-42BB-91EE-735614455405}" name="Table4" displayName="Table4" ref="A1:D35" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A1:D35" xr:uid="{8B5B2D93-E296-4982-9188-1B1EA292AE95}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D8">
     <sortCondition ref="A2:A8"/>
     <sortCondition ref="B2:B8"/>
@@ -4427,8 +6818,8 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5361,19 +7752,19 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B55" s="33" t="s">
         <v>218</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D55" s="14">
         <v>0</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -5390,7 +7781,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5409,50 +7800,74 @@
         <v>7</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
-        <v>227</v>
       </c>
       <c r="B2" s="18">
         <v>1</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="18">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="27"/>
+      <c r="A5" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="27"/>
+      <c r="A6" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="27"/>
+      <c r="A7" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" s="18">
+        <v>1</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="25"/>
@@ -5477,15 +7892,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87E8A4C-DD19-471A-8655-5F20C6D67CEA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
-    <col min="3" max="3" width="255.625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.5" style="31" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5497,88 +7912,118 @@
         <v>2</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B2" s="18">
         <v>1</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B4" s="18">
         <v>3</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B5" s="18"/>
+        <v>226</v>
+      </c>
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
       <c r="C5" s="21" t="s">
-        <v>232</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B6" s="18"/>
+        <v>226</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2</v>
+      </c>
       <c r="C6" s="21" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B7" s="18"/>
+        <v>226</v>
+      </c>
+      <c r="B7" s="18">
+        <v>3</v>
+      </c>
       <c r="C7" s="21" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="36"/>
+      <c r="A8" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="38">
+        <v>1</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="36"/>
+      <c r="A9" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="38">
+        <v>2</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="36"/>
+      <c r="A10" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="38">
+        <v>1</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="21"/>
+      <c r="A11" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="38">
+        <v>2</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="40"/>
@@ -5597,10 +8042,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F42A22B-36CC-4810-BF3A-03B3869F0BF4}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5608,7 +8053,7 @@
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
     <col min="3" max="3" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="164.625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="173.125" style="31" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5620,115 +8065,419 @@
         <v>3</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" s="18"/>
+      <c r="A2" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="18">
+        <v>2</v>
+      </c>
       <c r="C2" s="7"/>
       <c r="D2" s="27" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
-        <v>227</v>
-      </c>
-      <c r="B3" s="18"/>
+      <c r="A3" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="18">
+        <v>3</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="27" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="18">
+        <v>2</v>
+      </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="27"/>
+      <c r="D4" s="27" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2.5</v>
+      </c>
       <c r="C5" s="7"/>
-      <c r="D5" s="27"/>
+      <c r="D5" s="27" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" s="18">
+        <v>3</v>
+      </c>
       <c r="C6" s="7"/>
-      <c r="D6" s="27"/>
+      <c r="D6" s="27" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="18">
+        <v>3.5</v>
+      </c>
       <c r="C7" s="7"/>
-      <c r="D7" s="27"/>
+      <c r="D7" s="27" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="18">
+        <v>2</v>
+      </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="27"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="18"/>
+      <c r="D8" s="27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2.5</v>
+      </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="27"/>
+      <c r="D9" s="27" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="25"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="28"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="28"/>
+      <c r="A10" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="18">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="27" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" s="18">
+        <v>2</v>
+      </c>
       <c r="C12" s="25"/>
-      <c r="D12" s="28"/>
+      <c r="D12" s="28" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="18">
+        <v>2.5</v>
+      </c>
       <c r="C13" s="25"/>
-      <c r="D13" s="28"/>
+      <c r="D13" s="28" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" s="18">
+        <v>3</v>
+      </c>
       <c r="C14" s="25"/>
-      <c r="D14" s="28"/>
+      <c r="D14" s="28" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="B15" s="18">
+        <v>3.5</v>
+      </c>
       <c r="C15" s="25"/>
-      <c r="D15" s="27"/>
+      <c r="D15" s="28" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="25"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" s="18">
+        <v>2</v>
+      </c>
       <c r="C16" s="25"/>
-      <c r="D16" s="28"/>
+      <c r="D16" s="28" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="25"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2.5</v>
+      </c>
       <c r="C17" s="25"/>
-      <c r="D17" s="27"/>
+      <c r="D17" s="28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="B18" s="18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="28" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" s="18">
+        <v>2</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="28" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B21" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22" s="18">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="28" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B23" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" s="18">
+        <v>2</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="28" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B25" s="18">
+        <v>3</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="28" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B26" s="18">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="27" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B27" s="18">
+        <v>3</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="27" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="B28" s="18">
+        <v>2</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="B29" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="28" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" s="18">
+        <v>3</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="27" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B31" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="27" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="B32" s="18">
+        <v>2</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B33" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="27" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B34" s="18">
+        <v>3</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="27" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="B35" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="C35" s="25"/>
+      <c r="D35" s="27" t="s">
+        <v>269</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5743,8 +8492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA072BA0-A74B-4D64-9677-E60E9F767C6E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5752,7 +8501,7 @@
     <col min="1" max="1" width="15.75" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="177" style="31" customWidth="1"/>
+    <col min="4" max="4" width="183.75" style="31" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5772,41 +8521,73 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>227</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="30"/>
+      <c r="A3" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="36"/>
+      <c r="A4" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="36"/>
+      <c r="A5" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="39"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="21"/>
+      <c r="A6" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="37"/>

</xml_diff>

<commit_message>
[CN] EP16 : Abnormal Spectrum (H-Stage)
</commit_message>
<xml_diff>
--- a/temp/temp.xlsx
+++ b/temp/temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AN-EN-Tags\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CF1667-6DF4-48BD-A565-392E89D80860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5425712-6DD7-4E20-84EE-59CE9E504166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KW" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="277">
   <si>
     <t>Op</t>
   </si>
@@ -4143,6 +4143,15 @@
       </rPr>
       <t xml:space="preserve"> dodge when ammo is at or below half of ammo capacity</t>
     </r>
+  </si>
+  <si>
+    <t>; In &lt;@ba.kw&gt;[Sui's Garden of Grotesqueries]&lt;/&gt;, can attack additional target.</t>
+  </si>
+  <si>
+    <t>Can use up to 5 summons (max 3 deployed at once). Summons’ effect changes based upon Skill; In &lt;@ba.kw&gt;[Sui's Garden of Grotesqueries]&lt;/&gt;, retrieve summon in the 4 adjacent tiles, recover {} HP and attack deal addition {} ATK% as Arts damage (up to {} times)</t>
+  </si>
+  <si>
+    <t>Can use up to 5 summons (max 3 deployed at once). Summons’ effect changes based upon Skill; In &lt;@ba.kw&gt;[Sui's Garden of Grotesqueries]&lt;/&gt;, retrieve summon in the 4 adjacent tiles, recover {} HP and each attack deal addition {} ATK% as Arts damage (up to {} times)</t>
   </si>
 </sst>
 </file>
@@ -7068,8 +7077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F42A22B-36CC-4810-BF3A-03B3869F0BF4}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7509,17 +7518,21 @@
       <c r="C32" s="25"/>
       <c r="D32" s="28"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="18"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="27"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="27" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="18"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="27"/>
+      <c r="D34" s="27" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="25"/>
@@ -7540,8 +7553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA072BA0-A74B-4D64-9677-E60E9F767C6E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7601,7 +7614,9 @@
       <c r="A5" s="39"/>
       <c r="B5" s="7"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="42"/>
+      <c r="D5" s="42" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="39"/>

</xml_diff>